<commit_message>
Prepare infrastructure for financial statements (finStats) and start working on the reporting feature.
</commit_message>
<xml_diff>
--- a/financialStatements/finStatID_register.xlsx
+++ b/financialStatements/finStatID_register.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="17">
   <si>
     <t>guestListID_register</t>
   </si>
@@ -34,6 +34,9 @@
     <t>G2021042005</t>
   </si>
   <si>
+    <t>G2021092002</t>
+  </si>
+  <si>
     <t>F2021042004</t>
   </si>
   <si>
@@ -53,6 +56,9 @@
   </si>
   <si>
     <t>F2021042007</t>
+  </si>
+  <si>
+    <t>F2021092001</t>
   </si>
   <si>
     <t>1</t>
@@ -416,7 +422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -441,10 +447,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -455,10 +461,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -469,10 +475,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -483,10 +489,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -497,10 +503,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -511,10 +517,10 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -525,10 +531,10 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -539,10 +545,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -553,10 +559,10 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -567,10 +573,10 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -581,10 +587,10 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -595,10 +601,10 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -609,10 +615,10 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -623,10 +629,10 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -637,10 +643,10 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -651,10 +657,10 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -665,10 +671,10 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -679,10 +685,24 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
         <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>